<commit_message>
continue to work with dell
</commit_message>
<xml_diff>
--- a/config/SignalPlotStyleSpec.xlsx
+++ b/config/SignalPlotStyleSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjianhai/02_ADAS/01_repo/01_Tools/01_matlab/01_kpi_extractor/AEB_KPI_Project/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD7D6FD-5299-5C42-9E90-87265DF6F542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CDC791-61A4-4D4D-A741-76A807A3CFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="2540" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38360" yWindow="5400" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VbRcSignals" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
   <si>
     <t>A2LName</t>
   </si>
@@ -141,13 +141,175 @@
   </si>
   <si>
     <t>SteerAngle</t>
+  </si>
+  <si>
+    <t>Output_name</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Min_Axis_value</t>
+  </si>
+  <si>
+    <t>Max_Axis_value</t>
+  </si>
+  <si>
+    <t>Axis_Name</t>
+  </si>
+  <si>
+    <t>Condition_Var</t>
+  </si>
+  <si>
+    <t>Calibration_Lim</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>Veh_Spd</t>
+  </si>
+  <si>
+    <t>Vehicle Speed [kph]</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Vehicle Speed</t>
+  </si>
+  <si>
+    <t>Dead_Time</t>
+  </si>
+  <si>
+    <t>M1_DeadTime</t>
+  </si>
+  <si>
+    <t>Time [sec]</t>
+  </si>
+  <si>
+    <t>Cond_true</t>
+  </si>
+  <si>
+    <t>Dead Time</t>
+  </si>
+  <si>
+    <t>Intervention_Duration</t>
+  </si>
+  <si>
+    <t>Veh_Stop_Check</t>
+  </si>
+  <si>
+    <t>Intervention Duration</t>
+  </si>
+  <si>
+    <t>Maximum_Throttle_Value</t>
+  </si>
+  <si>
+    <t>Pedal_Max</t>
+  </si>
+  <si>
+    <t>PedalPos [%]</t>
+  </si>
+  <si>
+    <t>is_Pedal_Pressed_at_Start</t>
+  </si>
+  <si>
+    <t>PedalPosProIncrease_Th</t>
+  </si>
+  <si>
+    <t>Maximum Throttle Value</t>
+  </si>
+  <si>
+    <t>Maximum_Steering_Angle_Value</t>
+  </si>
+  <si>
+    <t>Abs_Steer_Max_deg</t>
+  </si>
+  <si>
+    <t>Steering_Angle [rad]</t>
+  </si>
+  <si>
+    <t>SteeringWheelAngle_Th</t>
+  </si>
+  <si>
+    <t>Maximum Steering Angle</t>
+  </si>
+  <si>
+    <t>Maximum_Steering_Rate_Value</t>
+  </si>
+  <si>
+    <t>Abs_Steer_Rate_Max_deg</t>
+  </si>
+  <si>
+    <t>Steering_Angle_Rate [rad/s]</t>
+  </si>
+  <si>
+    <t>AEB_SteeringAngleRate_Override</t>
+  </si>
+  <si>
+    <t>Maximum Steering Angle Rate</t>
+  </si>
+  <si>
+    <t>Maximum_Yaw_Rate_Value</t>
+  </si>
+  <si>
+    <t>Abs_Yaw_Rate_Max_deg</t>
+  </si>
+  <si>
+    <t>Yaw_Rate [rad/s]</t>
+  </si>
+  <si>
+    <t>YawrateSuspension_Th</t>
+  </si>
+  <si>
+    <t>Maximum Yaw Rate</t>
+  </si>
+  <si>
+    <t>Maximum_Lat_Acceleration</t>
+  </si>
+  <si>
+    <t>Abs_Lat_Acc_Max</t>
+  </si>
+  <si>
+    <t>Lat_Acceleration [m/s2]</t>
+  </si>
+  <si>
+    <t>LateralAcceleration_th</t>
+  </si>
+  <si>
+    <t>Maxime Lateral Acceleration</t>
+  </si>
+  <si>
+    <t>Longitudinal_Clearance</t>
+  </si>
+  <si>
+    <t>Long_Clearance</t>
+  </si>
+  <si>
+    <t>Long_Clearance [m]</t>
+  </si>
+  <si>
+    <t>Longitudinal Clearance</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +333,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -217,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -230,6 +399,17 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,7 +727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -732,26 +912,388 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24310F59-1486-4F41-B3B7-AB25CE8F592D}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
+        <v>150</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>100</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>300</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>600</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
+        <v>40</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <v>6</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>5</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1943DE-263B-CE4F-869C-DE791D333F1F}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="9">
+        <v>0</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0.74099999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="D4" s="9">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="9">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="9">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0.184</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.55600000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="9">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.188</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="9">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.745</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.93300000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="9">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="C9" s="9">
+        <v>7.8E-2</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.184</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>